<commit_message>
-comment bug -window too large -mounting location selector
</commit_message>
<xml_diff>
--- a/templates/dev_templates/starter_template.xlsx
+++ b/templates/dev_templates/starter_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\mathcad_auto\templates\dev_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512BC8D9-9187-4839-B159-F5B377A8EEB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CAC088-FFAB-4CB8-A788-9F6572FEDB57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19196" xr2:uid="{9B97A033-A49C-4F03-8482-3DF783EAAC46}"/>
+    <workbookView xWindow="1440" yWindow="1019" windowWidth="17606" windowHeight="14087" xr2:uid="{9B97A033-A49C-4F03-8482-3DF783EAAC46}"/>
   </bookViews>
   <sheets>
     <sheet name="values" sheetId="1" r:id="rId1"/>
@@ -1096,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873E901D-60E5-4378-B586-84E02EFBE42E}">
   <dimension ref="A1:S824"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>